<commit_message>
Changed LQR sim file.
</commit_message>
<xml_diff>
--- a/NamMatlab/QRL/parameters.xlsx
+++ b/NamMatlab/QRL/parameters.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="18195" windowHeight="9270" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="18195" windowHeight="9270" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="51" sheetId="2" r:id="rId2"/>
     <sheet name="52" sheetId="3" r:id="rId3"/>
+    <sheet name="53" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
   <si>
     <t>filenumber</t>
   </si>
@@ -658,6 +659,221 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2.2300000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2.99E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.28500000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4.0000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>92.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B25"/>
     </sheetView>
@@ -669,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>